<commit_message>
add scale factor 4 results and improved scale factor 0.5
</commit_message>
<xml_diff>
--- a/Reports/data/Experiments parameters.xlsx
+++ b/Reports/data/Experiments parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zas11\Desktop\MobilityDB-in-Azure\Reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B29D6F-58CF-44D1-8EA5-5960196DA116}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79122200-4CB4-4C31-9511-467A33E26A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>BerlinMod Benchmark</t>
+  </si>
+  <si>
+    <t>Experiment Group</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>B4ms</t>
   </si>
 </sst>
 </file>
@@ -223,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -275,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,9 +498,10 @@
     <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,8 +514,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -518,8 +531,11 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -532,8 +548,11 @@
       <c r="D3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -546,8 +565,11 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -560,8 +582,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -574,8 +599,11 @@
       <c r="D6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -588,8 +616,11 @@
       <c r="D7">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -602,8 +633,11 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -616,8 +650,11 @@
       <c r="D9">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -630,8 +667,11 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -643,6 +683,179 @@
       </c>
       <c r="D11" t="s">
         <v>17</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>32</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>120</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>